<commit_message>
Fixing Observation Profile Descriptions and titles
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-ihe-sdc-ecc-Observation-code.xlsx
+++ b/output/StructureDefinition-ihe-sdc-ecc-Observation-code.xlsx
@@ -45,7 +45,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>IHE SDC/eCC on FHIR Observation</t>
+    <t>IHE SDC/eCC on FHIR Observation Code</t>
   </si>
   <si>
     <t>Status</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-10-14T12:55:27-04:00</t>
+    <t>2021-10-14T13:09:30-04:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>